<commit_message>
adding materials and water quality tables
</commit_message>
<xml_diff>
--- a/Rfigs/summaryFigures.xlsx
+++ b/Rfigs/summaryFigures.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="material_costs" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="wq_fig" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,21 +21,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+  <si>
+    <t xml:space="preserve">Material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesh Size(mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost per bag($)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material Cost($)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchased through</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plastic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.webstaurantstore.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biopolymer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.bese-products.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.amazon.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cotton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.colonyco.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cellulose </t>
+  </si>
+  <si>
+    <t xml:space="preserve">80$</t>
+  </si>
   <si>
     <t xml:space="preserve">Site</t>
   </si>
   <si>
-    <t xml:space="preserve">Avg Phosphorus
-(mg/L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg
- NH3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg
- pH</t>
+    <t xml:space="preserve">Avg Phosphorus (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg NH3  (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg pH</t>
   </si>
   <si>
     <t xml:space="preserve">Avg DO</t>
@@ -44,12 +86,10 @@
     <t xml:space="preserve">Avg Temp (C)</t>
   </si>
   <si>
-    <t xml:space="preserve">Avg Conductivity
-(uS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avg Nitrogen
-(mg/L)</t>
+    <t xml:space="preserve">Avg Conductivity (uS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg Nitrogen (mg/L)</t>
   </si>
   <si>
     <t xml:space="preserve">Avg Flow Rate (m/s)</t>
@@ -140,14 +180,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -168,6 +210,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,12 +255,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,15 +293,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -262,104 +317,90 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="2" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B3" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>240</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="2" t="n">
+        <v>17.78</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B5" s="2" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="B6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>35</v>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -378,14 +419,131 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>